<commit_message>
fix: dynamically handle buttons in quick reply templates
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="91">
   <si>
     <t>Template Id</t>
   </si>
@@ -31,7 +31,7 @@
     <t>Button Type</t>
   </si>
   <si>
-    <t>Button Text</t>
+    <t>Button1</t>
   </si>
   <si>
     <t>Language</t>
@@ -65,6 +65,12 @@
   </si>
   <si>
     <t>Sample for dynamic URl</t>
+  </si>
+  <si>
+    <t>Button2</t>
+  </si>
+  <si>
+    <t>Button3</t>
   </si>
   <si>
     <t>broadcast_v2</t>
@@ -148,7 +154,13 @@
     <t>Quick Reply</t>
   </si>
   <si>
-    <t>Great, Okay, Bad(3 diff buttons)</t>
+    <t>Great</t>
+  </si>
+  <si>
+    <t>Okay</t>
+  </si>
+  <si>
+    <t>Bad</t>
   </si>
   <si>
     <t>cod_c</t>
@@ -428,8 +440,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="36.86"/>
-    <col customWidth="1" min="3" max="3" width="20.57"/>
-    <col customWidth="1" min="4" max="4" width="65.0"/>
+    <col customWidth="1" min="3" max="3" width="35.0"/>
+    <col customWidth="1" min="4" max="4" width="84.14"/>
     <col customWidth="1" min="5" max="5" width="20.57"/>
     <col customWidth="1" min="6" max="6" width="26.71"/>
     <col customWidth="1" min="7" max="7" width="23.14"/>
@@ -495,55 +507,61 @@
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="2" ht="79.5" customHeight="1">
       <c r="A2" s="2">
         <v>6088599.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J2" s="3">
         <v>44358.0</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
       <c r="R2" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
@@ -563,51 +581,51 @@
         <v>6088595.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J3" s="3">
         <v>44358.0</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
       <c r="R3" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="S3" s="5"/>
       <c r="T3" s="5"/>
@@ -627,52 +645,56 @@
         <v>6088592.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J4" s="3">
         <v>44358.0</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
       <c r="R4" s="4"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
+      <c r="S4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
       <c r="W4" s="5"/>
@@ -689,51 +711,51 @@
         <v>6088591.0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J5" s="3">
         <v>44358.0</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
       <c r="R5" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="S5" s="5"/>
       <c r="T5" s="5"/>
@@ -753,49 +775,49 @@
         <v>6088590.0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J6" s="3">
         <v>44358.0</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
       <c r="R6" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="S6" s="5"/>
       <c r="T6" s="5"/>
@@ -815,51 +837,51 @@
         <v>6088586.0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J7" s="3">
         <v>44358.0</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
       <c r="R7" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="S7" s="5"/>
       <c r="T7" s="5"/>
@@ -879,55 +901,55 @@
         <v>6088584.0</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J8" s="3">
         <v>44358.0</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="S8" s="5"/>
       <c r="T8" s="5"/>
@@ -947,51 +969,51 @@
         <v>6088581.0</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J9" s="3">
         <v>44358.0</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
       <c r="R9" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="S9" s="5"/>
       <c r="T9" s="5"/>
@@ -1011,55 +1033,55 @@
         <v>6088580.0</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J10" s="3">
         <v>44358.0</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="Q10" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="S10" s="5"/>
       <c r="T10" s="5"/>
@@ -1079,49 +1101,49 @@
         <v>23414.0</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="J11" s="3">
         <v>44358.0</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
       <c r="R11" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="S11" s="5"/>
       <c r="T11" s="5"/>
@@ -1141,55 +1163,55 @@
         <v>23413.0</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="J12" s="3">
         <v>44358.0</v>
       </c>
       <c r="K12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="P12" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="L12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="P12" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="Q12" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="S12" s="5"/>
       <c r="T12" s="5"/>
@@ -1209,51 +1231,51 @@
         <v>23412.0</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="J13" s="3">
         <v>44358.0</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
       <c r="R13" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="S13" s="5"/>
       <c r="T13" s="5"/>
@@ -1273,55 +1295,55 @@
         <v>23411.0</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="J14" s="3">
         <v>44358.0</v>
       </c>
       <c r="K14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="P14" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="L14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="O14" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="P14" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="Q14" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="R14" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="S14" s="5"/>
       <c r="T14" s="5"/>
@@ -1341,51 +1363,51 @@
         <v>23410.0</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="J15" s="3">
         <v>44358.0</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
       <c r="R15" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="S15" s="5"/>
       <c r="T15" s="5"/>
@@ -1405,40 +1427,40 @@
         <v>6089010.0</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J16" s="9">
         <v>44361.0</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
@@ -1463,40 +1485,40 @@
         <v>23652.0</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="J17" s="9">
         <v>44361.0</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>

</xml_diff>

<commit_message>
fix: add input optimisation in template automation
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tanul/Desktop/Bitspeed/gupshupTemplateApprover-/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Bitespeed\gupshupTemplateApprover-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61726E0-F6C6-2E40-B626-FA3A0337840D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE39F7E0-1B39-4A3E-9B41-5B8256961FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{6BD179F8-8D85-9F46-9907-3BA9FA31B970}"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="28800" windowHeight="15375" xr2:uid="{6BD179F8-8D85-9F46-9907-3BA9FA31B970}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,15 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -276,12 +267,6 @@
     <t>broadcast with image with quick reply</t>
   </si>
   <si>
-    <t>Tweet! Tweet! {{1}}, 
-We have an update for you. - {{2}}
-Chat with customer support at {{3}} (Click on CONTINUE button below 👇 to see customer support link).
-To unsubscribe from messages, please type STOP.</t>
-  </si>
-  <si>
     <t>Tweet! Tweet! {{1}}, Thanks!
 Your order is being prepared, we will let you know once it's ready. You can view the status of your order by clicking on the link below 👇
 Need to chat with us? Click here: {{4}}
@@ -368,6 +353,12 @@
     <t>Tweet! Tweet! {{1}}, 
 We have an update. Please click on yes below if you'd like us to share it with you.
 Chat with customer support at {{2}} (Click on CONTINUE button below 👇 to see customer support link).
+To unsubscribe from messages, please type STOP.</t>
+  </si>
+  <si>
+    <t>Tweet! Tweet! {{1}},
+We have an update for you. - {{2}}
+Chat with customer support at {{3}} (Click on CONTINUE button below 👇 to see customer support link).
 To unsubscribe from messages, please type STOP.</t>
   </si>
 </sst>
@@ -766,14 +757,14 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="34.1640625" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="34.125" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.625" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
     <col min="4" max="4" width="49.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -835,7 +826,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>6088599</v>
       </c>
@@ -846,7 +837,7 @@
         <v>21</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>22</v>
@@ -887,7 +878,7 @@
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
     </row>
-    <row r="3" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>6088595</v>
       </c>
@@ -898,7 +889,7 @@
         <v>33</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>34</v>
@@ -941,7 +932,7 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
     </row>
-    <row r="4" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>6088592</v>
       </c>
@@ -952,7 +943,7 @@
         <v>39</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>22</v>
@@ -997,7 +988,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>6088591</v>
       </c>
@@ -1008,7 +999,7 @@
         <v>45</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>34</v>
@@ -1051,7 +1042,7 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>6088590</v>
       </c>
@@ -1062,7 +1053,7 @@
         <v>48</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>34</v>
@@ -1103,7 +1094,7 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6088586</v>
       </c>
@@ -1114,7 +1105,7 @@
         <v>51</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>22</v>
@@ -1157,7 +1148,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6088584</v>
       </c>
@@ -1168,7 +1159,7 @@
         <v>54</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>22</v>
@@ -1215,7 +1206,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>6088581</v>
       </c>
@@ -1226,7 +1217,7 @@
         <v>58</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>22</v>
@@ -1269,7 +1260,7 @@
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
     </row>
-    <row r="10" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>6088580</v>
       </c>
@@ -1280,7 +1271,7 @@
         <v>60</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>22</v>
@@ -1327,7 +1318,7 @@
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
     </row>
-    <row r="11" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>23414</v>
       </c>
@@ -1338,7 +1329,7 @@
         <v>63</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>22</v>
@@ -1379,7 +1370,7 @@
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
     </row>
-    <row r="12" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>23413</v>
       </c>
@@ -1390,7 +1381,7 @@
         <v>67</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>22</v>
@@ -1437,7 +1428,7 @@
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
     </row>
-    <row r="13" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>23412</v>
       </c>
@@ -1448,7 +1439,7 @@
         <v>69</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>22</v>
@@ -1491,7 +1482,7 @@
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
     </row>
-    <row r="14" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>23411</v>
       </c>
@@ -1502,7 +1493,7 @@
         <v>71</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>22</v>
@@ -1549,7 +1540,7 @@
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
     </row>
-    <row r="15" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>23410</v>
       </c>
@@ -1560,7 +1551,7 @@
         <v>74</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>22</v>
@@ -1603,7 +1594,7 @@
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
     </row>
-    <row r="16" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>6089010</v>
       </c>
@@ -1614,7 +1605,7 @@
         <v>76</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>22</v>
@@ -1651,7 +1642,7 @@
       <c r="S16" s="2"/>
       <c r="T16" s="2"/>
     </row>
-    <row r="17" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>23652</v>
       </c>
@@ -1662,7 +1653,7 @@
         <v>79</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>22</v>
@@ -1699,7 +1690,7 @@
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
     </row>
-    <row r="18" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="N2" r:id="rId1" xr:uid="{2E26A896-1E52-7B46-95E1-727B72AF1E9E}"/>

</xml_diff>

<commit_message>
fix: force enable add-sample button in edge cases
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Bitespeed\gupshupTemplateApprover-\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tanul/Desktop/Bitspeed/gupshupTemplateApprover-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE39F7E0-1B39-4A3E-9B41-5B8256961FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4603E9D-4D64-044F-B06C-C53DCB143F70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="28800" windowHeight="15375" xr2:uid="{6BD179F8-8D85-9F46-9907-3BA9FA31B970}"/>
+    <workbookView xWindow="0" yWindow="1600" windowWidth="28800" windowHeight="15380" xr2:uid="{6BD179F8-8D85-9F46-9907-3BA9FA31B970}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -87,9 +87,6 @@
     <t>Button3</t>
   </si>
   <si>
-    <t>broadcast_v2</t>
-  </si>
-  <si>
     <t>broadcast without image with call action</t>
   </si>
   <si>
@@ -123,9 +120,6 @@
     <t>https://bspd.me/track</t>
   </si>
   <si>
-    <t>order_r2</t>
-  </si>
-  <si>
     <t>order receipt</t>
   </si>
   <si>
@@ -141,9 +135,6 @@
     <t>Azani</t>
   </si>
   <si>
-    <t>reordering_c</t>
-  </si>
-  <si>
     <t>reordering campaign</t>
   </si>
   <si>
@@ -159,36 +150,24 @@
     <t>Bad</t>
   </si>
   <si>
-    <t>cod_c</t>
-  </si>
-  <si>
     <t>cod confirmation</t>
   </si>
   <si>
     <t>Confirm Order</t>
   </si>
   <si>
-    <t>shipping_n</t>
-  </si>
-  <si>
     <t>shipping</t>
   </si>
   <si>
     <t>Track Order Status</t>
   </si>
   <si>
-    <t>browse_nd</t>
-  </si>
-  <si>
     <t>browse without image without discount</t>
   </si>
   <si>
     <t>Complete Payment</t>
   </si>
   <si>
-    <t>browse_d</t>
-  </si>
-  <si>
     <t>browse without image with discount</t>
   </si>
   <si>
@@ -198,24 +177,15 @@
     <t>code</t>
   </si>
   <si>
-    <t>abandon_nd</t>
-  </si>
-  <si>
     <t>abandon without image without discount</t>
   </si>
   <si>
-    <t>abandon_d</t>
-  </si>
-  <si>
     <t>abandon without image with discount</t>
   </si>
   <si>
     <t>5% off</t>
   </si>
   <si>
-    <t>broadcast_v2_img</t>
-  </si>
-  <si>
     <t>broadcast with image with call action</t>
   </si>
   <si>
@@ -225,43 +195,25 @@
     <t>INELIGIBLE</t>
   </si>
   <si>
-    <t>browse_img_d</t>
-  </si>
-  <si>
     <t>browse with image with discount</t>
   </si>
   <si>
-    <t>browse_img_nd</t>
-  </si>
-  <si>
     <t>browse with image wihtout discount</t>
   </si>
   <si>
-    <t>abandon_image_d</t>
-  </si>
-  <si>
     <t>adandon with image with discount</t>
   </si>
   <si>
     <t xml:space="preserve">code </t>
   </si>
   <si>
-    <t>abandon_img_nd</t>
-  </si>
-  <si>
     <t>abandon with image without discount</t>
   </si>
   <si>
-    <t>broadcast_v1</t>
-  </si>
-  <si>
     <t>broadcast without image with quick reply</t>
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>broadcast_img_v1</t>
   </si>
   <si>
     <t>broadcast with image with quick reply</t>
@@ -360,6 +312,54 @@
 We have an update for you. - {{2}}
 Chat with customer support at {{3}} (Click on CONTINUE button below 👇 to see customer support link).
 To unsubscribe from messages, please type STOP.</t>
+  </si>
+  <si>
+    <t>abandon_d_1</t>
+  </si>
+  <si>
+    <t>broadcast_v2_1</t>
+  </si>
+  <si>
+    <t>order_r2_1</t>
+  </si>
+  <si>
+    <t>reordering_c_1</t>
+  </si>
+  <si>
+    <t>cod_c_1</t>
+  </si>
+  <si>
+    <t>shipping_n_1</t>
+  </si>
+  <si>
+    <t>browse_nd_1</t>
+  </si>
+  <si>
+    <t>browse_d_1</t>
+  </si>
+  <si>
+    <t>abandon_nd_1</t>
+  </si>
+  <si>
+    <t>broadcast_v2_img_1</t>
+  </si>
+  <si>
+    <t>browse_img_d_1</t>
+  </si>
+  <si>
+    <t>browse_img_nd_1</t>
+  </si>
+  <si>
+    <t>abandon_image_d_1</t>
+  </si>
+  <si>
+    <t>abandon_img_nd_1</t>
+  </si>
+  <si>
+    <t>broadcast_v1_1</t>
+  </si>
+  <si>
+    <t>broadcast_img_v1_1</t>
   </si>
 </sst>
 </file>
@@ -369,7 +369,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -395,6 +395,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -419,10 +427,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -437,8 +446,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -754,17 +765,17 @@
   <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="34.125" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="34.1640625" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.625" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
     <col min="4" max="4" width="49.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -826,813 +837,813 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>6088599</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="J2" s="3">
         <v>44358</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
-      <c r="R2" s="4" t="s">
-        <v>31</v>
+      <c r="R2" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
     </row>
-    <row r="3" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>6088595</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="F3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="H3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="J3" s="3">
         <v>44358</v>
       </c>
       <c r="K3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="M3" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
     </row>
-    <row r="4" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>6088592</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="H4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="J4" s="3">
         <v>44358</v>
       </c>
       <c r="K4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="M4" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="4"/>
       <c r="S4" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>6088591</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="J5" s="3">
         <v>44358</v>
       </c>
       <c r="K5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L5" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="M5" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>6088590</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="J6" s="3">
         <v>44358</v>
       </c>
       <c r="K6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L6" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="M6" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6088586</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="G7" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="J7" s="3">
         <v>44358</v>
       </c>
       <c r="K7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L7" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="M7" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>6088584</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="J8" s="3">
         <v>44358</v>
       </c>
       <c r="K8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L8" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="M8" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="Q8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R8" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="R8" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>6088581</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="G9" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="J9" s="3">
         <v>44358</v>
       </c>
       <c r="K9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L9" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="M9" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
     </row>
-    <row r="10" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>6088580</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="G10" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="J10" s="3">
         <v>44358</v>
       </c>
       <c r="K10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L10" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="M10" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="Q10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R10" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="R10" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
     </row>
-    <row r="11" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>23414</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="I11" s="2" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="J11" s="3">
         <v>44358</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="L11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="N11" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
     </row>
-    <row r="12" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>23413</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="G12" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="J12" s="3">
         <v>44358</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="Q12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R12" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="R12" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
     </row>
-    <row r="13" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>23412</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="G13" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="J13" s="3">
         <v>44358</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
     </row>
-    <row r="14" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>23411</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>87</v>
-      </c>
       <c r="E14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="G14" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="J14" s="3">
         <v>44358</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="Q14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R14" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="R14" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
     </row>
-    <row r="15" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>23410</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="G15" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="J15" s="3">
         <v>44358</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
     </row>
-    <row r="16" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>6089010</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>92</v>
-      </c>
       <c r="E16" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="H16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="J16" s="6">
         <v>44361</v>
       </c>
       <c r="K16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L16" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="M16" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
@@ -1642,45 +1653,45 @@
       <c r="S16" s="2"/>
       <c r="T16" s="2"/>
     </row>
-    <row r="17" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>23652</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="J17" s="6">
         <v>44361</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
@@ -1690,7 +1701,7 @@
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
     </row>
-    <row r="18" spans="1:20" ht="78.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:20" ht="79" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="N2" r:id="rId1" xr:uid="{2E26A896-1E52-7B46-95E1-727B72AF1E9E}"/>

</xml_diff>